<commit_message>
Make auto formatting/convert configurable and support rationals
</commit_message>
<xml_diff>
--- a/spec/data/SpecNumberFormat.xlsx
+++ b/spec/data/SpecNumberFormat.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Test</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>0123.50</t>
+  </si>
+  <si>
+    <t>0123</t>
   </si>
 </sst>
 </file>
@@ -111,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -125,6 +131,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,96 +445,122 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="9">
-        <v>123</v>
-      </c>
-      <c r="C3" s="1" t="str">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13" t="str">
+        <f>Sheet2!A2</f>
+        <v>0123</v>
+      </c>
+      <c r="C3" s="4" t="str">
         <f>Sheet2!$A$1</f>
         <v>Test</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5">
-        <v>123</v>
-      </c>
-      <c r="C4" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13" t="str">
+        <f>Sheet2!A3</f>
+        <v>0123.50</v>
+      </c>
+      <c r="C4" s="4" t="str">
         <f>Sheet2!$A$1</f>
         <v>Test</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>25569</v>
-      </c>
-      <c r="C5" s="3" t="str">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9">
+        <v>123</v>
+      </c>
+      <c r="C5" s="1" t="str">
         <f>Sheet2!$A$1</f>
         <v>Test</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="12">
-        <v>42048.527835648143</v>
-      </c>
-      <c r="C6" s="6" t="str">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <v>123</v>
+      </c>
+      <c r="C6" s="5" t="str">
         <f>Sheet2!$A$1</f>
         <v>Test</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.99990000000000001</v>
-      </c>
-      <c r="C7" s="2" t="str">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>25569</v>
+      </c>
+      <c r="C7" s="3" t="str">
         <f>Sheet2!$A$1</f>
         <v>Test</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="C8" s="7" t="str">
+        <v>5</v>
+      </c>
+      <c r="B8" s="12">
+        <v>42048.527835648143</v>
+      </c>
+      <c r="C8" s="6" t="str">
         <f>Sheet2!$A$1</f>
         <v>Test</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10">
-        <v>3.4028236692093801E+38</v>
-      </c>
-      <c r="C9" s="10" t="str">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="C9" s="2" t="str">
         <f>Sheet2!$A$1</f>
         <v>Test</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="7" t="str">
+        <f>Sheet2!$A$1</f>
+        <v>Test</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="10">
+        <v>3.4028236692093801E+38</v>
+      </c>
+      <c r="C11" s="10" t="str">
+        <f>Sheet2!$A$1</f>
+        <v>Test</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B12" s="11">
         <v>123</v>
       </c>
-      <c r="C10" s="11" t="str">
+      <c r="C12" s="11" t="str">
         <f>Sheet2!$A$1</f>
         <v>Test</v>
       </c>
@@ -540,10 +573,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,7 +586,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>